<commit_message>
updated soft-bottom habitat health and resilience and pressure layers
</commit_message>
<xml_diff>
--- a/prep/HAB/NOAA_benthic_scores.xlsx
+++ b/prep/HAB/NOAA_benthic_scores.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,29 +395,32 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>60.893999999999998</v>
+        <v>70.278111111111116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>70.278111111111116</v>
+        <v>60.138666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>60.138666666666666</v>
+        <v>60.893999999999998</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B5">
+    <sortCondition ref="A2:A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>